<commit_message>
Update Parents attendance form for first term exam.xlsx
</commit_message>
<xml_diff>
--- a/Parents attendence form in first term exam.xlsx
+++ b/Parents attendence form in first term exam.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\first term 2082\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DECB0C9-2845-4D27-99AB-6D6129AAD80B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA1A57A-4CA7-4D99-9A77-9A34734D3C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="8" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="16" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ten" sheetId="1" r:id="rId1"/>
@@ -28,13 +28,18 @@
     <sheet name="2 wood" sheetId="14" r:id="rId13"/>
     <sheet name="1, sibia" sheetId="15" r:id="rId14"/>
     <sheet name="1 peacock" sheetId="16" r:id="rId15"/>
+    <sheet name="Nursery danfe" sheetId="17" r:id="rId16"/>
+    <sheet name="Nursery Dove" sheetId="18" r:id="rId17"/>
+    <sheet name="Lkg Kite" sheetId="19" r:id="rId18"/>
+    <sheet name="uKG PARROT" sheetId="20" r:id="rId19"/>
+    <sheet name="UKG,SPARROW" sheetId="21" r:id="rId20"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="580">
   <si>
     <t>Roll</t>
   </si>
@@ -1288,6 +1293,492 @@
   </si>
   <si>
     <t>Class: One Peacock, Parents Attendence Form, First Terminal Examination 2082</t>
+  </si>
+  <si>
+    <t>AARAV BOGATI</t>
+  </si>
+  <si>
+    <t>AARON ARYAL</t>
+  </si>
+  <si>
+    <t>ABHI DARAI</t>
+  </si>
+  <si>
+    <t>ALISHA CHAUDHARY</t>
+  </si>
+  <si>
+    <t>ADRIAN CHAUDHARY</t>
+  </si>
+  <si>
+    <t>AIKA CHAUDHARY</t>
+  </si>
+  <si>
+    <t>AMAN BAHADUR GURUNG</t>
+  </si>
+  <si>
+    <t>BHABYA CHAUDHARY</t>
+  </si>
+  <si>
+    <t>DEVANSH MAHATO</t>
+  </si>
+  <si>
+    <t>ERIN MAHATO</t>
+  </si>
+  <si>
+    <t>EVANSH MAHATO</t>
+  </si>
+  <si>
+    <t>EVEREST CHAUDHARY</t>
+  </si>
+  <si>
+    <t>MAYARA TAMANG</t>
+  </si>
+  <si>
+    <t>PRIYAL THAPA</t>
+  </si>
+  <si>
+    <t>RAJESHA KHADKA</t>
+  </si>
+  <si>
+    <t>REJOICE CHAUDHARY</t>
+  </si>
+  <si>
+    <t>RIDIMA MAHATO</t>
+  </si>
+  <si>
+    <t>RIKRINA MAHATO</t>
+  </si>
+  <si>
+    <t>RIYANSHU CHAUDHARY</t>
+  </si>
+  <si>
+    <t>ROHIT MAHATO</t>
+  </si>
+  <si>
+    <t>SAIMAN TAMANG</t>
+  </si>
+  <si>
+    <t>SANISH PARIYAR</t>
+  </si>
+  <si>
+    <t>SANVI SUBEDI</t>
+  </si>
+  <si>
+    <t>SHUBHAM MAHATO</t>
+  </si>
+  <si>
+    <t>SIMRAN SILWAL</t>
+  </si>
+  <si>
+    <t>SUJAL RAM</t>
+  </si>
+  <si>
+    <t>SUSHAMI KHAREL</t>
+  </si>
+  <si>
+    <t>WILLIAM GURUNG</t>
+  </si>
+  <si>
+    <t>YUBIKA GURUNG</t>
+  </si>
+  <si>
+    <t>Class: Nursery Danfe, Parents Attendence Form, First Terminal Examination 2082</t>
+  </si>
+  <si>
+    <t>AADITYA NARAYAN SHRESTHA</t>
+  </si>
+  <si>
+    <t>AAILA RAI</t>
+  </si>
+  <si>
+    <t>ALIJA MAHATO</t>
+  </si>
+  <si>
+    <t>ASIM CHAUDHARY</t>
+  </si>
+  <si>
+    <t>BINESH TAMANG</t>
+  </si>
+  <si>
+    <t>BINISHA CHAUDHARY THARU</t>
+  </si>
+  <si>
+    <t>BIVAN KUMAL</t>
+  </si>
+  <si>
+    <t>BRANSON CHAUDHARY</t>
+  </si>
+  <si>
+    <t>DIBINSH CHAUDHARY</t>
+  </si>
+  <si>
+    <t>ELAZNA CHAUDHARY</t>
+  </si>
+  <si>
+    <t>HIMANI TAMANG</t>
+  </si>
+  <si>
+    <t>JERUSHA SUNAR</t>
+  </si>
+  <si>
+    <t>KARTIK CHAUDHARY</t>
+  </si>
+  <si>
+    <t>KARTIK THAKUR</t>
+  </si>
+  <si>
+    <t>KEYARIN CHAUDHARY</t>
+  </si>
+  <si>
+    <t>LABISH KUMAL</t>
+  </si>
+  <si>
+    <t>LUCKY SHRESTHA</t>
+  </si>
+  <si>
+    <t>MEDRIX CHAUDHARY</t>
+  </si>
+  <si>
+    <t>NEMAT KHATUN</t>
+  </si>
+  <si>
+    <t>PRAVESH TAMANG</t>
+  </si>
+  <si>
+    <t>PRIYANS MAHATO</t>
+  </si>
+  <si>
+    <t>RAYNISH CHAUDHARY</t>
+  </si>
+  <si>
+    <t>RIYANSH CHAUDHARY</t>
+  </si>
+  <si>
+    <t>RIYASA MAHATO</t>
+  </si>
+  <si>
+    <t>RIYASHNA MAHATO</t>
+  </si>
+  <si>
+    <t>SANVI CHAUDHARY</t>
+  </si>
+  <si>
+    <t>SAYUNA CHHETRI</t>
+  </si>
+  <si>
+    <t>SHICHAN SHRESTHA</t>
+  </si>
+  <si>
+    <t>SHREEYANSH MAHATO</t>
+  </si>
+  <si>
+    <t>SUJATA BOTE</t>
+  </si>
+  <si>
+    <t>SUJIN MAHATO</t>
+  </si>
+  <si>
+    <t>SUVANSH MAHATO</t>
+  </si>
+  <si>
+    <t>YUNSANG TAMANG</t>
+  </si>
+  <si>
+    <t>DARSHAN BHUSAL</t>
+  </si>
+  <si>
+    <t>Class: Nursery Dove Parents Attendence Form, First Terminal Examination 2082</t>
+  </si>
+  <si>
+    <t>Class: LKG, Kite Parents Attendence Form, First Terminal Examination 2082</t>
+  </si>
+  <si>
+    <t>AALISKA MAHATO</t>
+  </si>
+  <si>
+    <t>AARONS MAHATO</t>
+  </si>
+  <si>
+    <t>AARUSH CHAUDHARY</t>
+  </si>
+  <si>
+    <t>AAYUSHA BOTE</t>
+  </si>
+  <si>
+    <t>ANISH TAMANG</t>
+  </si>
+  <si>
+    <t>ANSHUL CHAUDHARY</t>
+  </si>
+  <si>
+    <t>ARADHANA KARNA</t>
+  </si>
+  <si>
+    <t>ARIKA SILWAL</t>
+  </si>
+  <si>
+    <t>AROSHANG TAMANG</t>
+  </si>
+  <si>
+    <t>BINISHA KUMAL</t>
+  </si>
+  <si>
+    <t>ERIC TAMANG</t>
+  </si>
+  <si>
+    <t>NABAYUG SHAH</t>
+  </si>
+  <si>
+    <t>NAIRA MAHATO</t>
+  </si>
+  <si>
+    <t>PRANISH ARYAL</t>
+  </si>
+  <si>
+    <t>PRATIK TAMANG</t>
+  </si>
+  <si>
+    <t>REETI SAPKOTA</t>
+  </si>
+  <si>
+    <t>REHAN PARIYAR</t>
+  </si>
+  <si>
+    <t>RENSY MAHATO</t>
+  </si>
+  <si>
+    <t>SAMIR TAMANG</t>
+  </si>
+  <si>
+    <t>SAMRAT SAPKOTA</t>
+  </si>
+  <si>
+    <t>SANISH TAMANG</t>
+  </si>
+  <si>
+    <t>SANJIT DARAI</t>
+  </si>
+  <si>
+    <t>SARANSH PAKHRIN</t>
+  </si>
+  <si>
+    <t>SAYDRINA CHAUDHARY</t>
+  </si>
+  <si>
+    <t>SHREEJU THARU</t>
+  </si>
+  <si>
+    <t>SHREEYA MAHATO</t>
+  </si>
+  <si>
+    <t>SHREYAN KUMAL</t>
+  </si>
+  <si>
+    <t>SIMON POUDEL</t>
+  </si>
+  <si>
+    <t>SUYOG MAHATO</t>
+  </si>
+  <si>
+    <t>TIA MAHATO</t>
+  </si>
+  <si>
+    <t>YASBIN SARU MAGAR</t>
+  </si>
+  <si>
+    <t>YUVAN KHANAL</t>
+  </si>
+  <si>
+    <t>SHREEYANSHI CHAUDHARY</t>
+  </si>
+  <si>
+    <t>Class: UKG Parrot Parents Attendence Form, First Terminal Examination 2082</t>
+  </si>
+  <si>
+    <t>AAYUSMA TAMANG</t>
+  </si>
+  <si>
+    <t>ANSHUMAN KUMAL</t>
+  </si>
+  <si>
+    <t>ANUJ DARAI</t>
+  </si>
+  <si>
+    <t>ANUSKA KUMARI CHAUDHAR</t>
+  </si>
+  <si>
+    <t>ASHISH ROKA</t>
+  </si>
+  <si>
+    <t>AYAM MAHATO</t>
+  </si>
+  <si>
+    <t>BRYAN CHAUDHARY</t>
+  </si>
+  <si>
+    <t>CHAHANA PULAMI MAGAR</t>
+  </si>
+  <si>
+    <t>JASON SHRESTHA</t>
+  </si>
+  <si>
+    <t>KRISTIN MAHATO</t>
+  </si>
+  <si>
+    <t>MESAK CHAUDHARY</t>
+  </si>
+  <si>
+    <t>NIBISHA BAJAGAI</t>
+  </si>
+  <si>
+    <t>NIRJAL PARIYAR</t>
+  </si>
+  <si>
+    <t>NISCHAL MAHATO</t>
+  </si>
+  <si>
+    <t>PREETI KUMARI YADAV</t>
+  </si>
+  <si>
+    <t>PRINSIKA KUMARI</t>
+  </si>
+  <si>
+    <t>RAYHAN KHATIWADA</t>
+  </si>
+  <si>
+    <t>REEWAZ SAPKOTA</t>
+  </si>
+  <si>
+    <t>RITIK CHAUDHARY</t>
+  </si>
+  <si>
+    <t>RIYANSHI TAMANG</t>
+  </si>
+  <si>
+    <t>ROHISHA PARIYAR</t>
+  </si>
+  <si>
+    <t>RONAM RAUT</t>
+  </si>
+  <si>
+    <t>SAMIR POUDEL</t>
+  </si>
+  <si>
+    <t>SARANSH DARAI</t>
+  </si>
+  <si>
+    <t>SHISON TAMANG</t>
+  </si>
+  <si>
+    <t>SHRISH REGMI</t>
+  </si>
+  <si>
+    <t>SUJAL DONG</t>
+  </si>
+  <si>
+    <t>SUSHANT BC</t>
+  </si>
+  <si>
+    <t>SUYOG NEUPANE</t>
+  </si>
+  <si>
+    <t>MANA KUMARI PRAJA</t>
+  </si>
+  <si>
+    <t>Class: UKG SPARROW Parents Attendence Form, First Terminal Examination 2082</t>
+  </si>
+  <si>
+    <t>AABISHKA MAHATO</t>
+  </si>
+  <si>
+    <t>AAGAM GHIMIRE</t>
+  </si>
+  <si>
+    <t>AAHANA DARAI</t>
+  </si>
+  <si>
+    <t>AARADHYA CHAUDHARY</t>
+  </si>
+  <si>
+    <t>AARYANSH CHAUDHARY</t>
+  </si>
+  <si>
+    <t>AAYAN BOTE</t>
+  </si>
+  <si>
+    <t>AAYARA LAMA</t>
+  </si>
+  <si>
+    <t>ANSONSH ARYAL</t>
+  </si>
+  <si>
+    <t>ARISHA MAHATO</t>
+  </si>
+  <si>
+    <t>ASWIN CHAPAGAI</t>
+  </si>
+  <si>
+    <t>BINAYASH CHAUDHARY</t>
+  </si>
+  <si>
+    <t>BIYANKA BAMJAN</t>
+  </si>
+  <si>
+    <t>DHIRAJ MAHATO</t>
+  </si>
+  <si>
+    <t>FRANCESCA CHAUDHARY</t>
+  </si>
+  <si>
+    <t>HENU RAI</t>
+  </si>
+  <si>
+    <t>LIYANA CHAUDHARY</t>
+  </si>
+  <si>
+    <t>NIRISHA CHAUDHARY</t>
+  </si>
+  <si>
+    <t>PRASIDDHI CHAPAGAIN</t>
+  </si>
+  <si>
+    <t>PRATHANA SAPKOTA</t>
+  </si>
+  <si>
+    <t>RIYAJ MAHATO</t>
+  </si>
+  <si>
+    <t>RONISHA MAHATO</t>
+  </si>
+  <si>
+    <t>SAMARTHA DAHAL</t>
+  </si>
+  <si>
+    <t>SAMIKSHA SHRESTHA</t>
+  </si>
+  <si>
+    <t>SANIDYA SAPKOTA</t>
+  </si>
+  <si>
+    <t>SARINA CHAUDHARY</t>
+  </si>
+  <si>
+    <t>SHIVAM THAKUR</t>
+  </si>
+  <si>
+    <t>SHIVANSH RAUT</t>
+  </si>
+  <si>
+    <t>SHREEYAS POKHREL</t>
+  </si>
+  <si>
+    <t>SWOSTIKA KUMAL</t>
+  </si>
+  <si>
+    <t>URGEN TAMANG</t>
+  </si>
+  <si>
+    <t>VISION MAHATO</t>
   </si>
 </sst>
 </file>
@@ -1342,7 +1833,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1499,13 +1990,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1552,6 +2056,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3728,8 +4237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01DC50FB-0892-4680-83F0-91653F2E42AE}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4042,6 +4551,1498 @@
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C3ACE72-1C05-41BE-B263-234DDFCDD4FA}">
+  <dimension ref="A1:D31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="24" customHeight="1">
+      <c r="A1" s="33" t="s">
+        <v>447</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+    </row>
+    <row r="2" spans="1:4" ht="24" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="24" customHeight="1">
+      <c r="A3" s="35">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="C3" s="34"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" ht="24" customHeight="1">
+      <c r="A4" s="35">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="C4" s="34"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" ht="24" customHeight="1">
+      <c r="A5" s="35">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="C5" s="34"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" ht="24" customHeight="1">
+      <c r="A6" s="35">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="C6" s="34"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" ht="24" customHeight="1">
+      <c r="A7" s="35">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="C7" s="34"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="24" customHeight="1">
+      <c r="A8" s="35">
+        <v>5</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="C8" s="34"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" ht="24" customHeight="1">
+      <c r="A9" s="35">
+        <v>6</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="C9" s="34"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" ht="24" customHeight="1">
+      <c r="A10" s="35">
+        <v>7</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" ht="24" customHeight="1">
+      <c r="A11" s="35">
+        <v>8</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="C11" s="34"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" ht="24" customHeight="1">
+      <c r="A12" s="35">
+        <v>9</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="C12" s="34"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" ht="24" customHeight="1">
+      <c r="A13" s="35">
+        <v>10</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="C13" s="34"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" ht="24" customHeight="1">
+      <c r="A14" s="35">
+        <v>11</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="C14" s="34"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" ht="24" customHeight="1">
+      <c r="A15" s="35">
+        <v>12</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="C15" s="34"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" ht="24" customHeight="1">
+      <c r="A16" s="35">
+        <v>13</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="C16" s="34"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" ht="24" customHeight="1">
+      <c r="A17" s="35">
+        <v>14</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="C17" s="34"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" ht="24" customHeight="1">
+      <c r="A18" s="35">
+        <v>15</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="C18" s="34"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" ht="24" customHeight="1">
+      <c r="A19" s="35">
+        <v>16</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="C19" s="34"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" ht="24" customHeight="1">
+      <c r="A20" s="35">
+        <v>17</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="C20" s="34"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" ht="24" customHeight="1">
+      <c r="A21" s="35">
+        <v>18</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="C21" s="34"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" ht="24" customHeight="1">
+      <c r="A22" s="35">
+        <v>19</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="C22" s="34"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" ht="24" customHeight="1">
+      <c r="A23" s="35">
+        <v>20</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="C23" s="34"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" ht="24" customHeight="1">
+      <c r="A24" s="35">
+        <v>21</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="C24" s="34"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" ht="24" customHeight="1">
+      <c r="A25" s="35">
+        <v>22</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="C25" s="34"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" ht="24" customHeight="1">
+      <c r="A26" s="35">
+        <v>23</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="C26" s="34"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" ht="24" customHeight="1">
+      <c r="A27" s="35">
+        <v>24</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="C27" s="34"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" ht="24" customHeight="1">
+      <c r="A28" s="35">
+        <v>25</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="C28" s="34"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" ht="24" customHeight="1">
+      <c r="A29" s="35">
+        <v>26</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="C29" s="34"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A30" s="35">
+        <v>27</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="C30" s="34"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" ht="22.5" customHeight="1">
+      <c r="A31" s="35">
+        <v>28</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A2D4E1C-C8A6-4112-8D5E-DD72707BB5CC}">
+  <dimension ref="A1:D36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="24" customHeight="1">
+      <c r="A1" s="33" t="s">
+        <v>482</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="21" customHeight="1">
+      <c r="A3" s="35">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="C3" s="34"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" ht="21" customHeight="1">
+      <c r="A4" s="35">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="C4" s="34"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" ht="21" customHeight="1">
+      <c r="A5" s="35">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="C5" s="34"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" ht="21" customHeight="1">
+      <c r="A6" s="35">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="C6" s="34"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" ht="21" customHeight="1">
+      <c r="A7" s="35">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="C7" s="34"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="21" customHeight="1">
+      <c r="A8" s="35">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="C8" s="34"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" ht="21" customHeight="1">
+      <c r="A9" s="35">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="C9" s="34"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" ht="21" customHeight="1">
+      <c r="A10" s="35">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" ht="21" customHeight="1">
+      <c r="A11" s="35">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="C11" s="34"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" ht="21" customHeight="1">
+      <c r="A12" s="35">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="C12" s="34"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" ht="21" customHeight="1">
+      <c r="A13" s="35">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="C13" s="34"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" ht="21" customHeight="1">
+      <c r="A14" s="35">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="C14" s="34"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" ht="21" customHeight="1">
+      <c r="A15" s="35">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="C15" s="34"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" ht="21" customHeight="1">
+      <c r="A16" s="35">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="C16" s="34"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" ht="21" customHeight="1">
+      <c r="A17" s="35">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="C17" s="34"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" ht="21" customHeight="1">
+      <c r="A18" s="35">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="C18" s="34"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" ht="21" customHeight="1">
+      <c r="A19" s="35">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="C19" s="34"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" ht="21" customHeight="1">
+      <c r="A20" s="35">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="C20" s="34"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" ht="21" customHeight="1">
+      <c r="A21" s="35">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="C21" s="34"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" ht="21" customHeight="1">
+      <c r="A22" s="35">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="C22" s="34"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" ht="21" customHeight="1">
+      <c r="A23" s="35">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="C23" s="34"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" ht="21" customHeight="1">
+      <c r="A24" s="35">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="C24" s="34"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" ht="21" customHeight="1">
+      <c r="A25" s="35">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="C25" s="34"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" ht="21" customHeight="1">
+      <c r="A26" s="35">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="C26" s="34"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" ht="21" customHeight="1">
+      <c r="A27" s="35">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="C27" s="34"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" ht="21" customHeight="1">
+      <c r="A28" s="35">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="C28" s="34"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" ht="21" customHeight="1">
+      <c r="A29" s="35">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="C29" s="34"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" ht="21" customHeight="1">
+      <c r="A30" s="35">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="C30" s="34"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" ht="21" customHeight="1">
+      <c r="A31" s="35">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="C31" s="34"/>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" ht="21" customHeight="1">
+      <c r="A32" s="35">
+        <v>31</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" ht="21" customHeight="1">
+      <c r="A33" s="35">
+        <v>32</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" ht="21" customHeight="1">
+      <c r="A34" s="35">
+        <v>33</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" ht="21" customHeight="1">
+      <c r="A35" s="35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" ht="21" customHeight="1">
+      <c r="A36" s="36">
+        <v>36</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A888C8E0-18AC-478C-A397-87334CA1C6D5}">
+  <dimension ref="A1:D37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="24" customHeight="1">
+      <c r="A1" s="33" t="s">
+        <v>483</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+    </row>
+    <row r="2" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A3" s="35">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="C3" s="34"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A4" s="35">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="C4" s="34"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A5" s="35">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="C5" s="34"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A6" s="35">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="C6" s="34"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A7" s="35">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="C7" s="34"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A8" s="35">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="C8" s="34"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A9" s="35">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="C9" s="34"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A10" s="35">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A11" s="35">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="C11" s="34"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A12" s="35">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="C12" s="34"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A13" s="35">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="C13" s="34"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A14" s="35">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="C14" s="34"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A15" s="35">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="C15" s="34"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A16" s="35">
+        <v>14</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="C16" s="34"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A17" s="35">
+        <v>15</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="C17" s="34"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A18" s="35">
+        <v>16</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="C18" s="34"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A19" s="35">
+        <v>17</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="C19" s="34"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A20" s="35">
+        <v>18</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="C20" s="34"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A21" s="35">
+        <v>19</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="C21" s="34"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A22" s="35">
+        <v>20</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="C22" s="34"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A23" s="35">
+        <v>21</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="C23" s="34"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A24" s="35">
+        <v>22</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="C24" s="34"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A25" s="35">
+        <v>23</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="C25" s="34"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A26" s="35">
+        <v>24</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>506</v>
+      </c>
+      <c r="C26" s="34"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A27" s="35">
+        <v>25</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>507</v>
+      </c>
+      <c r="C27" s="34"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A28" s="35">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>508</v>
+      </c>
+      <c r="C28" s="34"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A29" s="35">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>509</v>
+      </c>
+      <c r="C29" s="34"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A30" s="35">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="C30" s="34"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A31" s="35">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C31" s="34"/>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A32" s="35">
+        <v>31</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="C32" s="34"/>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A33" s="35">
+        <v>32</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="C33" s="34"/>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A34" s="35">
+        <v>33</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>513</v>
+      </c>
+      <c r="C34" s="34"/>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A35" s="35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>514</v>
+      </c>
+      <c r="C35" s="34"/>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A36" s="35">
+        <v>35</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="C36" s="34"/>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A37" s="35">
+        <v>36</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>516</v>
+      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C43206-63A7-44F1-9702-DA07C42D21A9}">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="24" customHeight="1">
+      <c r="A1" s="33" t="s">
+        <v>517</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+    </row>
+    <row r="2" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A3" s="35">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A4" s="35">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>519</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A5" s="35">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>520</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A6" s="35">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A7" s="35">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>522</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A8" s="35">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A9" s="35">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A10" s="35">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>525</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A11" s="35">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A12" s="35">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>527</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A13" s="35">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>528</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A14" s="35">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>529</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A15" s="35">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A16" s="35">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>531</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A17" s="35">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>532</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A18" s="35">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>533</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A19" s="35">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>534</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A20" s="35">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A21" s="35">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A22" s="35">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A23" s="35">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>538</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A24" s="35">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>539</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A25" s="35">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A26" s="35">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>540</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A27" s="35">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A28" s="35">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>541</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A29" s="35">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A30" s="35">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>543</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A31" s="35">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>544</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A32" s="35">
+        <v>31</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>545</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A33" s="35">
+        <v>32</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A34" s="35">
+        <v>33</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4330,6 +6331,374 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BF9DBD3-76FF-4514-A972-73CD2DD4395C}">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="24" customHeight="1">
+      <c r="A1" s="33" t="s">
+        <v>548</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+    </row>
+    <row r="2" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A3" s="35">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A4" s="35">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A5" s="35">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>551</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A6" s="35">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>552</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A7" s="35">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A8" s="35">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>554</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A9" s="35">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A10" s="35">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A11" s="35">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>557</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A12" s="35">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>558</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A13" s="35">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A14" s="35">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A15" s="35">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>561</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A16" s="35">
+        <v>14</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A17" s="35">
+        <v>15</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A18" s="35">
+        <v>16</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>563</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A19" s="35">
+        <v>17</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A20" s="35">
+        <v>18</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>565</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A21" s="35">
+        <v>19</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>566</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A22" s="35">
+        <v>20</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>567</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A23" s="35">
+        <v>21</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>568</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A24" s="35">
+        <v>22</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>569</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A25" s="35">
+        <v>23</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>570</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A26" s="35">
+        <v>24</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>571</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A27" s="35">
+        <v>25</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>572</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A28" s="35">
+        <v>26</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>573</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A29" s="35">
+        <v>27</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A30" s="35">
+        <v>28</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>575</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A31" s="35">
+        <v>29</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A32" s="35">
+        <v>30</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>577</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A33" s="35">
+        <v>31</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A34" s="35">
+        <v>32</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65CE3F45-4C43-4CB3-A7E7-5EA50835CD3F}">
   <dimension ref="A1:D27"/>

</xml_diff>